<commit_message>
Changes to model, and fixed bug causing incorrect scaling for OTH model display
</commit_message>
<xml_diff>
--- a/python/Data/poll-data-fed.xlsx
+++ b/python/Data/poll-data-fed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\python\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A359F8BD-DDEA-4C40-BDED-7584A30EB575}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3481C9E8-309F-4FB6-B6FC-86B0F34BE5DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4335" yWindow="3090" windowWidth="25095" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="4275" windowWidth="27375" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -107,7 +107,7 @@
     <t>F2F Morgan</t>
   </si>
   <si>
-    <t>L_NP FP</t>
+    <t>LNP FP</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="600" activePane="bottomLeft"/>
       <selection activeCell="B1" sqref="B1:B1048576"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update poll data and spreadsheets
</commit_message>
<xml_diff>
--- a/python/Data/poll-data-fed.xlsx
+++ b/python/Data/poll-data-fed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\python\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B922C83-A1DC-4D1B-BB49-4D5FE094BB26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F75513E-5978-4BA6-80B6-8673DBD819E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="2625" windowWidth="13380" windowHeight="16845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="4245" windowWidth="19425" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="23">
   <si>
     <t>MidDate</t>
   </si>
@@ -422,12 +422,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V1164"/>
+  <dimension ref="A1:V1167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A1131" activePane="bottomLeft"/>
+      <pane ySplit="600" topLeftCell="A1143" activePane="bottomLeft"/>
       <selection activeCell="K1" sqref="K1:V1048576"/>
-      <selection pane="bottomLeft" activeCell="H1150" sqref="H1150"/>
+      <selection pane="bottomLeft" activeCell="L1156" sqref="L1156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12995,14 +12995,14 @@
       <c r="C369">
         <v>56</v>
       </c>
-      <c r="D369">
-        <v>0</v>
-      </c>
-      <c r="E369">
-        <v>0</v>
-      </c>
-      <c r="F369">
-        <v>0</v>
+      <c r="D369" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E369" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F369" t="e">
+        <v>#N/A</v>
       </c>
       <c r="G369" t="e">
         <v>#N/A</v>
@@ -13013,8 +13013,8 @@
       <c r="I369" t="e">
         <v>#N/A</v>
       </c>
-      <c r="J369">
-        <v>0</v>
+      <c r="J369" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L369" s="2"/>
       <c r="N369" s="1"/>
@@ -15605,22 +15605,22 @@
     </row>
     <row r="446" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A446" s="1">
-        <v>40380</v>
+        <v>40379</v>
       </c>
       <c r="B446" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C446">
-        <v>55.5</v>
+        <v>54</v>
       </c>
       <c r="D446">
-        <v>38.5</v>
+        <v>41</v>
       </c>
       <c r="E446">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F446">
-        <v>11.5</v>
+        <v>12</v>
       </c>
       <c r="G446" t="e">
         <v>#N/A</v>
@@ -15632,29 +15632,29 @@
         <v>#N/A</v>
       </c>
       <c r="J446">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L446" s="2"/>
       <c r="N446" s="1"/>
     </row>
     <row r="447" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A447" s="1">
-        <v>40379</v>
+        <v>40380</v>
       </c>
       <c r="B447" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C447">
-        <v>54</v>
+        <v>55.5</v>
       </c>
       <c r="D447">
-        <v>41</v>
+        <v>38.5</v>
       </c>
       <c r="E447">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F447">
-        <v>12</v>
+        <v>11.5</v>
       </c>
       <c r="G447" t="e">
         <v>#N/A</v>
@@ -15666,7 +15666,7 @@
         <v>#N/A</v>
       </c>
       <c r="J447">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L447" s="2"/>
       <c r="N447" s="1"/>
@@ -15741,22 +15741,22 @@
     </row>
     <row r="450" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A450" s="1">
-        <v>40387</v>
+        <v>40384</v>
       </c>
       <c r="B450" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C450">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D450">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E450">
-        <v>42</v>
+        <v>43.5</v>
       </c>
       <c r="F450">
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="G450" t="e">
         <v>#N/A</v>
@@ -15768,29 +15768,29 @@
         <v>#N/A</v>
       </c>
       <c r="J450">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L450" s="2"/>
       <c r="N450" s="1"/>
     </row>
     <row r="451" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A451" s="1">
-        <v>40384</v>
+        <v>40386</v>
       </c>
       <c r="B451" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C451">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D451">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E451">
-        <v>43.5</v>
+        <v>36</v>
       </c>
       <c r="F451">
-        <v>11.5</v>
+        <v>12</v>
       </c>
       <c r="G451" t="e">
         <v>#N/A</v>
@@ -15802,29 +15802,29 @@
         <v>#N/A</v>
       </c>
       <c r="J451">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L451" s="2"/>
       <c r="N451" s="1"/>
     </row>
     <row r="452" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A452" s="1">
-        <v>40386</v>
+        <v>40387</v>
       </c>
       <c r="B452" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C452">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D452">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E452">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F452">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G452" t="e">
         <v>#N/A</v>
@@ -15836,7 +15836,7 @@
         <v>#N/A</v>
       </c>
       <c r="J452">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L452" s="2"/>
       <c r="N452" s="1"/>
@@ -40035,6 +40035,102 @@
       </c>
       <c r="J1164">
         <v>7.5</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1165" s="1">
+        <v>44141</v>
+      </c>
+      <c r="B1165" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1165">
+        <v>49</v>
+      </c>
+      <c r="D1165">
+        <v>43</v>
+      </c>
+      <c r="E1165">
+        <v>35</v>
+      </c>
+      <c r="F1165">
+        <v>11</v>
+      </c>
+      <c r="G1165">
+        <v>3</v>
+      </c>
+      <c r="H1165" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I1165" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J1165">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1166" s="1">
+        <v>44153</v>
+      </c>
+      <c r="B1166" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1166">
+        <v>49.5</v>
+      </c>
+      <c r="D1166">
+        <v>42</v>
+      </c>
+      <c r="E1166">
+        <v>34</v>
+      </c>
+      <c r="F1166">
+        <v>12</v>
+      </c>
+      <c r="G1166">
+        <v>4</v>
+      </c>
+      <c r="H1166" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I1166" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J1166">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1167" s="1">
+        <v>44162</v>
+      </c>
+      <c r="B1167" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1167">
+        <v>49</v>
+      </c>
+      <c r="D1167">
+        <v>43</v>
+      </c>
+      <c r="E1167">
+        <v>36</v>
+      </c>
+      <c r="F1167">
+        <v>11</v>
+      </c>
+      <c r="G1167">
+        <v>2</v>
+      </c>
+      <c r="H1167" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I1167" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J1167">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Simulations now take results from the last day of the projection. Also, adjusted model code to give even less weight to priors.
</commit_message>
<xml_diff>
--- a/python/Data/poll-data-fed.xlsx
+++ b/python/Data/poll-data-fed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\python\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F75513E-5978-4BA6-80B6-8673DBD819E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFDDEB2-824D-4916-AB9F-1204C85CCEFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="4245" windowWidth="19425" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1005" yWindow="4005" windowWidth="31245" windowHeight="15690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="23">
   <si>
     <t>MidDate</t>
   </si>
@@ -422,12 +422,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V1167"/>
+  <dimension ref="A1:V1168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="600" topLeftCell="A1143" activePane="bottomLeft"/>
       <selection activeCell="K1" sqref="K1:V1048576"/>
-      <selection pane="bottomLeft" activeCell="L1156" sqref="L1156"/>
+      <selection pane="bottomLeft" activeCell="F1153" sqref="F1153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40133,6 +40133,38 @@
         <v>8</v>
       </c>
     </row>
+    <row r="1168" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1168" s="1">
+        <v>44225</v>
+      </c>
+      <c r="B1168" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1168">
+        <v>50</v>
+      </c>
+      <c r="D1168">
+        <v>42</v>
+      </c>
+      <c r="E1168">
+        <v>36</v>
+      </c>
+      <c r="F1168">
+        <v>10</v>
+      </c>
+      <c r="G1168">
+        <v>3</v>
+      </c>
+      <c r="H1168" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I1168" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J1168">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add clear all button for results, other misc changes
Misc changes: reduce number of iterations for adjusting
poll trend from 5000 to 1000 to save calculation time,
update for new niv/nsw elections in pystan model,
add output for start/end date of model before calculation
so it can be checked that the latest poll updates are
properly included, update with latest polls
</commit_message>
<xml_diff>
--- a/python/Data/poll-data-fed.xlsx
+++ b/python/Data/poll-data-fed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\python\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED11039-0C64-425A-B9CA-F8DDDF6AF856}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D104C92-2C99-4D51-AB84-AAAB3BEB3A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6030" yWindow="5280" windowWidth="30180" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17580" yWindow="2625" windowWidth="19755" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="24">
   <si>
     <t>MidDate</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Morgan Phone</t>
+  </si>
+  <si>
+    <t>ResolvePM</t>
   </si>
 </sst>
 </file>
@@ -430,12 +433,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:V1176"/>
+  <dimension ref="A1:V1186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A1165" activePane="bottomLeft"/>
+      <pane ySplit="600" topLeftCell="A1168" activePane="bottomLeft"/>
       <selection activeCell="C1" sqref="C1:J1048576"/>
-      <selection pane="bottomLeft" activeCell="H1173" sqref="H1173"/>
+      <selection pane="bottomLeft" activeCell="E1188" sqref="E1188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40428,7 +40431,318 @@
         <v>#N/A</v>
       </c>
       <c r="J1176" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1177" s="1">
+        <v>44267</v>
+      </c>
+      <c r="B1177" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1177" s="3">
+        <v>52</v>
+      </c>
+      <c r="D1177" s="3">
+        <v>39</v>
+      </c>
+      <c r="E1177" s="3">
+        <v>39</v>
+      </c>
+      <c r="F1177" s="3">
         <v>10</v>
+      </c>
+      <c r="G1177" s="3">
+        <v>3</v>
+      </c>
+      <c r="H1177" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I1177" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J1177" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1178" s="1">
+        <v>44265</v>
+      </c>
+      <c r="B1178" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1178" s="3">
+        <v>50.5</v>
+      </c>
+      <c r="D1178" s="3">
+        <v>41</v>
+      </c>
+      <c r="E1178" s="3">
+        <v>34.5</v>
+      </c>
+      <c r="F1178" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="G1178" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="H1178" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I1178" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J1178" s="3">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1179" s="1">
+        <v>44281</v>
+      </c>
+      <c r="B1179" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1179" s="3">
+        <v>52</v>
+      </c>
+      <c r="D1179" s="3">
+        <v>40</v>
+      </c>
+      <c r="E1179" s="3">
+        <v>38</v>
+      </c>
+      <c r="F1179" s="3">
+        <v>11</v>
+      </c>
+      <c r="G1179" s="3">
+        <v>2</v>
+      </c>
+      <c r="H1179" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I1179" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J1179" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1180" s="1">
+        <v>44303</v>
+      </c>
+      <c r="B1180" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1180" s="3">
+        <v>38</v>
+      </c>
+      <c r="E1180" s="3">
+        <v>33</v>
+      </c>
+      <c r="F1180" s="3">
+        <v>12</v>
+      </c>
+      <c r="G1180" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1180" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I1180" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J1180" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1181" s="1">
+        <v>44309</v>
+      </c>
+      <c r="B1181" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1181" s="3">
+        <v>51</v>
+      </c>
+      <c r="D1181" s="3">
+        <v>41</v>
+      </c>
+      <c r="E1181" s="3">
+        <v>38</v>
+      </c>
+      <c r="F1181" s="3">
+        <v>10</v>
+      </c>
+      <c r="G1181" s="3">
+        <v>3</v>
+      </c>
+      <c r="H1181" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I1181" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J1181" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1182" s="1">
+        <v>44331</v>
+      </c>
+      <c r="B1182" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1182" s="3">
+        <v>51</v>
+      </c>
+      <c r="D1182" s="3">
+        <v>41</v>
+      </c>
+      <c r="E1182" s="3">
+        <v>36</v>
+      </c>
+      <c r="F1182" s="3">
+        <v>12</v>
+      </c>
+      <c r="G1182" s="3">
+        <v>2</v>
+      </c>
+      <c r="H1182" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I1182" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J1182" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1183" s="1">
+        <v>44330</v>
+      </c>
+      <c r="B1183" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1183" s="3">
+        <v>39</v>
+      </c>
+      <c r="E1183" s="3">
+        <v>35</v>
+      </c>
+      <c r="F1183" s="3">
+        <v>12</v>
+      </c>
+      <c r="G1183" s="3">
+        <v>2</v>
+      </c>
+      <c r="H1183" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I1183" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J1183" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1184" s="1">
+        <v>44351</v>
+      </c>
+      <c r="B1184" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1184" s="3">
+        <v>50</v>
+      </c>
+      <c r="D1184" s="3">
+        <v>41</v>
+      </c>
+      <c r="E1184" s="3">
+        <v>36</v>
+      </c>
+      <c r="F1184" s="3">
+        <v>11</v>
+      </c>
+      <c r="G1184" s="3">
+        <v>3</v>
+      </c>
+      <c r="H1184" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I1184" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J1184" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1185" s="1">
+        <v>44349</v>
+      </c>
+      <c r="B1185" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1185" s="3">
+        <v>51</v>
+      </c>
+      <c r="D1185" s="3">
+        <v>40</v>
+      </c>
+      <c r="E1185" s="3">
+        <v>35.5</v>
+      </c>
+      <c r="F1185" s="3">
+        <v>11.5</v>
+      </c>
+      <c r="G1185" s="3">
+        <v>3</v>
+      </c>
+      <c r="H1185" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I1185" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J1185" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1186" s="1">
+        <v>44358</v>
+      </c>
+      <c r="B1186" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1186" s="3">
+        <v>40</v>
+      </c>
+      <c r="E1186" s="3">
+        <v>36</v>
+      </c>
+      <c r="F1186" s="3">
+        <v>10</v>
+      </c>
+      <c r="G1186" s="3">
+        <v>3</v>
+      </c>
+      <c r="H1186" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I1186" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J1186" s="3">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make stan model go back to previous election
Also, updates to poll data and analysis from recently published polls.
</commit_message>
<xml_diff>
--- a/python/Data/poll-data-fed.xlsx
+++ b/python/Data/poll-data-fed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\python\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D104C92-2C99-4D51-AB84-AAAB3BEB3A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813C9B26-7A33-408A-A4D8-467A027A84A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17580" yWindow="2625" windowWidth="19755" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17520" yWindow="6960" windowWidth="20130" windowHeight="13275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="24">
   <si>
     <t>MidDate</t>
   </si>
@@ -433,12 +433,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:V1186"/>
+  <dimension ref="A1:V1187"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="600" topLeftCell="A1168" activePane="bottomLeft"/>
       <selection activeCell="C1" sqref="C1:J1048576"/>
-      <selection pane="bottomLeft" activeCell="E1188" sqref="E1188"/>
+      <selection pane="bottomLeft" activeCell="D1180" sqref="D1180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40745,6 +40745,38 @@
         <v>12</v>
       </c>
     </row>
+    <row r="1187" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1187" s="1">
+        <v>44363</v>
+      </c>
+      <c r="B1187" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1187" s="3">
+        <v>50.5</v>
+      </c>
+      <c r="D1187" s="3">
+        <v>41.5</v>
+      </c>
+      <c r="E1187" s="3">
+        <v>34.5</v>
+      </c>
+      <c r="F1187" s="3">
+        <v>12</v>
+      </c>
+      <c r="G1187" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="H1187" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I1187" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J1187" s="3">
+        <v>8.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>